<commit_message>
tích hợp công thức từ option
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/GiaVatLieu.xlsx
+++ b/Worksheet/Content/Template/GiaVatLieu.xlsx
@@ -13,6 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Giá vật liệu" sheetId="1" r:id="rId1"/>
+    <sheet name="Cước biển" sheetId="5" r:id="rId2"/>
+    <sheet name="Cước TC" sheetId="4" r:id="rId3"/>
+    <sheet name="Cước ô tô" sheetId="2" r:id="rId4"/>
+    <sheet name="Cước sông" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -161,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -194,7 +198,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="hair">
+      <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -206,10 +210,38 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="hair">
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -218,20 +250,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -240,6 +264,14 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -248,6 +280,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,29 +576,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="B1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="15" width="14.5546875" customWidth="1"/>
-    <col min="16" max="16" width="15.109375" customWidth="1"/>
-    <col min="17" max="17" width="16.21875" customWidth="1"/>
-    <col min="18" max="18" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
+    <col min="3" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="44.21875" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="11" width="14.5546875" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="21" width="18" customWidth="1"/>
+    <col min="22" max="22" width="16.21875" customWidth="1"/>
+    <col min="23" max="23" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="2:23" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -573,13 +615,17 @@
       <c r="O1" s="15"/>
       <c r="P1" s="15"/>
       <c r="Q1" s="15"/>
-      <c r="R1" s="1"/>
-    </row>
-    <row r="2" spans="1:18" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -595,13 +641,17 @@
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -617,111 +667,344 @@
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
-      <c r="R3" s="1"/>
-    </row>
-    <row r="4" spans="1:18" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="2:23" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="5"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="11"/>
+    <row r="5" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+    </row>
+    <row r="6" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+    </row>
+    <row r="7" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+    </row>
+    <row r="8" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+    </row>
+    <row r="9" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+    </row>
+    <row r="10" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+    </row>
+    <row r="11" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+    </row>
+    <row r="12" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+    </row>
+    <row r="13" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+    </row>
+    <row r="14" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="5"/>
+    </row>
+    <row r="15" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="B1:V1"/>
+    <mergeCell ref="B2:V2"/>
+    <mergeCell ref="B3:V3"/>
   </mergeCells>
-  <conditionalFormatting sqref="G5:G6">
+  <conditionalFormatting sqref="K14:K15">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -729,4 +1012,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix lại công thức khi xóa cột
</commit_message>
<xml_diff>
--- a/Worksheet/Content/Template/GiaVatLieu.xlsx
+++ b/Worksheet/Content/Template/GiaVatLieu.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>BẢNG GIÁ VẬT LIỆU</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Cước ô tô</t>
-  </si>
-  <si>
-    <t>Cước ô tô mới</t>
   </si>
   <si>
     <t>Cước sông</t>
@@ -272,6 +269,15 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -280,15 +286,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,435 +573,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" customWidth="1"/>
-    <col min="3" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="44.21875" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
-    <col min="7" max="11" width="14.5546875" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="21" width="18" customWidth="1"/>
-    <col min="22" max="22" width="16.21875" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="44.21875" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="16.21875" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:17" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="1"/>
-    </row>
-    <row r="2" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="1"/>
-    </row>
-    <row r="3" spans="2:23" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="1"/>
-    </row>
-    <row r="4" spans="2:23" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="J4" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="V4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="W4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-    </row>
-    <row r="6" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="19"/>
-    </row>
-    <row r="7" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="19"/>
-    </row>
-    <row r="8" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="19"/>
-    </row>
-    <row r="9" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-    </row>
-    <row r="10" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-    </row>
-    <row r="11" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="19"/>
-    </row>
-    <row r="12" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="19"/>
-    </row>
-    <row r="13" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="20"/>
-      <c r="V13" s="20"/>
-      <c r="W13" s="20"/>
-    </row>
-    <row r="14" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="6"/>
+    </row>
+    <row r="5" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+    </row>
+    <row r="6" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+    </row>
+    <row r="7" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+    </row>
+    <row r="8" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+    </row>
+    <row r="9" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+    </row>
+    <row r="10" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+    </row>
+    <row r="11" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+    </row>
+    <row r="12" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+    </row>
+    <row r="13" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+    </row>
+    <row r="14" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="8"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="5"/>
-    </row>
-    <row r="15" spans="2:23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="12"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="12"/>
-      <c r="W15" s="11"/>
+      <c r="Q15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:V1"/>
-    <mergeCell ref="B2:V2"/>
-    <mergeCell ref="B3:V3"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A3:P3"/>
   </mergeCells>
-  <conditionalFormatting sqref="K14:K15">
+  <conditionalFormatting sqref="G14:G15">
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>